<commit_message>
added steps to require student set the seed
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/Topic2DQ1Template.xlsx
+++ b/144F20/Topic 2/Topic2DQ1Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\Offline\Course Materials\git\Teaching\144F20\Topic 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2831CAE7-2A0B-413A-880A-AC94D689AD7E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{9849C032-CAEF-42A3-9421-7CD7863FF371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="732" yWindow="732" windowWidth="20796" windowHeight="11424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="Richard Ketchersid - Personal View" guid="{E42251D7-B26D-493B-AB47-FC9D5E718532}" mergeInterval="0" personalView="1" xWindow="61" yWindow="61" windowWidth="1733" windowHeight="952" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Richard Ketchersid - Personal View" guid="{E42251D7-B26D-493B-AB47-FC9D5E718532}" mergeInterval="0" personalView="1" xWindow="61" yWindow="61" windowWidth="1733" windowHeight="952" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -619,7 +621,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -696,9 +700,6 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -749,12 +750,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -923,8 +937,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7F73379B-E737-4580-8C18-9CF0D1DE9E0F}">
-  <header guid="{7F73379B-E737-4580-8C18-9CF0D1DE9E0F}" dateTime="2020-09-25T14:19:12" maxSheetId="4" userName="Richard Ketchersid" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CAD98F8A-115D-4985-AB1A-B164582FA9A6}">
+  <header guid="{CAD98F8A-115D-4985-AB1A-B164582FA9A6}" dateTime="2020-11-14T12:16:54" maxSheetId="4" userName="Richard Ketchersid" r:id="rId1">
     <sheetIdMap count="3">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -939,7 +953,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{CAD98F8A-115D-4985-AB1A-B164582FA9A6}" name="Richard Ketchersid" id="-1739585321" dateTime="2020-11-14T12:16:54"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1208,7 +1224,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1224,20 +1240,20 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1"/>
     <row r="2" spans="1:8" ht="15" thickBot="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="27" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="43" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.6" thickTop="1" thickBot="1">
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="30"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
@@ -1272,7 +1288,7 @@
         <v>16.27</v>
       </c>
       <c r="C5" s="17"/>
-      <c r="D5" s="28"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="22"/>
       <c r="G5" s="4" t="s">
         <v>7</v>
@@ -1391,11 +1407,11 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="25" t="s">
         <v>41</v>
       </c>
@@ -1405,30 +1421,30 @@
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1"/>
     <row r="15" spans="1:8" ht="14.4" customHeight="1">
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="2:5" ht="15" thickBot="1">
-      <c r="B17" s="41"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="cDBi4K1q9fUFb7oIRgVnAbOmZJZBw7TO+Ax1OqphCANkkk0O3CieOElvYP4QYXJeLyVZ0b/1zwiwysDdmx25zA==" saltValue="hGHcc6ftYXI2QgQtid9zcg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0"/>
   <customSheetViews>
     <customSheetView guid="{E42251D7-B26D-493B-AB47-FC9D5E718532}">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H16" sqref="H16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -1439,13 +1455,18 @@
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="B15:E17"/>
   </mergeCells>
+  <conditionalFormatting sqref="A5:E12">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$D$2="Your Name"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="55" id="{E9611DED-43D1-4477-97E6-AED09D5C24E8}">
+          <x14:cfRule type="expression" priority="56" id="{E9611DED-43D1-4477-97E6-AED09D5C24E8}">
             <xm:f>AND(_xlfn.ISFORMULA(A7),ABS(A7-Solution!A7)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>
@@ -1455,7 +1476,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="43" id="{5F8CF386-A089-4D42-9F11-FDD5F2503D44}">
+          <x14:cfRule type="expression" priority="44" id="{5F8CF386-A089-4D42-9F11-FDD5F2503D44}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(A7)),ABS(A7-Solution!A7)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1468,7 +1489,7 @@
           <xm:sqref>A7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="19" id="{B05D6209-C902-4E1A-826F-7E0CD3A64E0C}">
+          <x14:cfRule type="expression" priority="20" id="{B05D6209-C902-4E1A-826F-7E0CD3A64E0C}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(A9)),ABS(A9-Solution!A9)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1478,7 +1499,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="20" id="{25EC0DCC-B6E5-4399-A6D7-786F5E13A611}">
+          <x14:cfRule type="expression" priority="21" id="{25EC0DCC-B6E5-4399-A6D7-786F5E13A611}">
             <xm:f>AND(_xlfn.ISFORMULA(A9),ABS(A9-Solution!A9)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>
@@ -1491,7 +1512,7 @@
           <xm:sqref>A9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="17" id="{37254A07-2A8D-4F6C-BA1E-EA0FD2B84316}">
+          <x14:cfRule type="expression" priority="18" id="{37254A07-2A8D-4F6C-BA1E-EA0FD2B84316}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(A11)),ABS(A11-Solution!A11)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1501,7 +1522,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="18" id="{E4BEF26F-727E-49BB-874B-972F03E3A1D7}">
+          <x14:cfRule type="expression" priority="19" id="{E4BEF26F-727E-49BB-874B-972F03E3A1D7}">
             <xm:f>AND(_xlfn.ISFORMULA(A11),ABS(A11-Solution!A11)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>
@@ -1514,7 +1535,7 @@
           <xm:sqref>A11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="15" id="{9C603ADB-1A96-41C3-84C5-BEC09EC1465F}">
+          <x14:cfRule type="expression" priority="16" id="{9C603ADB-1A96-41C3-84C5-BEC09EC1465F}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(B8)),ABS(B8-Solution!B8)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1524,7 +1545,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="16" id="{D1C24D64-71DF-4B6C-957F-D66AFA78B590}">
+          <x14:cfRule type="expression" priority="17" id="{D1C24D64-71DF-4B6C-957F-D66AFA78B590}">
             <xm:f>AND(_xlfn.ISFORMULA(B8),ABS(B8-Solution!B8)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>
@@ -1537,7 +1558,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="13" id="{269E3E59-A51D-4BE3-8885-D8BA05C1D63A}">
+          <x14:cfRule type="expression" priority="14" id="{269E3E59-A51D-4BE3-8885-D8BA05C1D63A}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(B10)),ABS(B10-Solution!B10)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1547,7 +1568,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="14" id="{8E744E33-0030-41D6-9A85-9F1F8934A0DF}">
+          <x14:cfRule type="expression" priority="15" id="{8E744E33-0030-41D6-9A85-9F1F8934A0DF}">
             <xm:f>AND(_xlfn.ISFORMULA(B10),ABS(B10-Solution!B10)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>
@@ -1560,7 +1581,7 @@
           <xm:sqref>B10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="11" id="{D5C10216-7341-4B19-9524-42040A5DD605}">
+          <x14:cfRule type="expression" priority="12" id="{D5C10216-7341-4B19-9524-42040A5DD605}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(B12)),ABS(B12-Solution!B12)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1570,7 +1591,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="12" id="{92B3A3B4-5051-46D5-A368-82F587CCC5FB}">
+          <x14:cfRule type="expression" priority="13" id="{92B3A3B4-5051-46D5-A368-82F587CCC5FB}">
             <xm:f>AND(_xlfn.ISFORMULA(B12),ABS(B12-Solution!B12)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>
@@ -1583,7 +1604,7 @@
           <xm:sqref>B12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="9" id="{953AC69A-F4AF-43F2-AE36-6E7095FA1E64}">
+          <x14:cfRule type="expression" priority="10" id="{953AC69A-F4AF-43F2-AE36-6E7095FA1E64}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(C9)),ABS(C9-Solution!C9)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1593,7 +1614,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="10" id="{1D0E7C80-DB20-404B-8665-01A1187C97FD}">
+          <x14:cfRule type="expression" priority="11" id="{1D0E7C80-DB20-404B-8665-01A1187C97FD}">
             <xm:f>AND(_xlfn.ISFORMULA(C9),ABS(C9-Solution!C9)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>
@@ -1606,7 +1627,7 @@
           <xm:sqref>C9:C12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="7" id="{1D43F37E-8E51-486D-92C5-27AA9DA152FD}">
+          <x14:cfRule type="expression" priority="8" id="{1D43F37E-8E51-486D-92C5-27AA9DA152FD}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(C5)),ABS(C5-Solution!C5)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1616,7 +1637,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="8" id="{9B74A47D-16BC-4AB0-BE1C-358D3A1174DF}">
+          <x14:cfRule type="expression" priority="9" id="{9B74A47D-16BC-4AB0-BE1C-358D3A1174DF}">
             <xm:f>AND(_xlfn.ISFORMULA(C5),ABS(C5-Solution!C5)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>
@@ -1629,7 +1650,7 @@
           <xm:sqref>C5:C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{F9AA9CCE-0BC9-4ED8-AC6D-E232A8CECC7C}">
+          <x14:cfRule type="expression" priority="6" id="{F9AA9CCE-0BC9-4ED8-AC6D-E232A8CECC7C}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(D5)),ABS(D5-Solution!D5)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1639,7 +1660,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="6" id="{7B7B5EE6-8899-4576-A6B1-42BFF0BD7E50}">
+          <x14:cfRule type="expression" priority="7" id="{7B7B5EE6-8899-4576-A6B1-42BFF0BD7E50}">
             <xm:f>AND(_xlfn.ISFORMULA(D5),ABS(D5-Solution!D5)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>
@@ -1652,7 +1673,7 @@
           <xm:sqref>D5:D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{9460091A-5324-4F81-B241-D4E901A1DC12}">
+          <x14:cfRule type="expression" priority="4" id="{9460091A-5324-4F81-B241-D4E901A1DC12}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(D11)),ABS(D11-Solution!D11)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1662,7 +1683,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="4" id="{B31CD53D-D4C9-459D-8E49-B20EF11BD29F}">
+          <x14:cfRule type="expression" priority="5" id="{B31CD53D-D4C9-459D-8E49-B20EF11BD29F}">
             <xm:f>AND(_xlfn.ISFORMULA(D11),ABS(D11-Solution!D11)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>
@@ -1675,7 +1696,7 @@
           <xm:sqref>D11:D12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{1AE492DD-50AC-4984-830A-0679E869B8C8}">
+          <x14:cfRule type="expression" priority="2" id="{1AE492DD-50AC-4984-830A-0679E869B8C8}">
             <xm:f>OR(NOT(_xlfn.ISFORMULA(E5)),ABS(E5-Solution!E5)&gt;0.00005)</xm:f>
             <x14:dxf>
               <font>
@@ -1685,7 +1706,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="2" id="{F4D92430-B5A7-4F88-A0AF-FB0FDFD65D87}">
+          <x14:cfRule type="expression" priority="3" id="{F4D92430-B5A7-4F88-A0AF-FB0FDFD65D87}">
             <xm:f>AND(_xlfn.ISFORMULA(E5),ABS(E5-Solution!E5)&lt;0.0005)</xm:f>
             <x14:dxf>
               <font>

</xml_diff>